<commit_message>
[UPDATE] Pred Var Names
</commit_message>
<xml_diff>
--- a/data/simple_200.xlsx
+++ b/data/simple_200.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisco/Git/sa-uta8-utaut/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D3BCC9-A79F-6C4E-8775-0AAFE51C5B2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B3299-C666-7D44-8BA3-9B8DF9A94409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,11 +397,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BD201"/>
+  <dimension ref="A1:AK201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>